<commit_message>
swaped hispaniola with jamaica
</commit_message>
<xml_diff>
--- a/data/Insula_checklist.xlsx
+++ b/data/Insula_checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Luis/Desktop/Caribbean_frogs/Insula_frog_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Luis/Desktop/RUG_IslandBiology_MScCourse/Practicals/DAISIE_Insula_beetles/0.Insula_beetle_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB38EA9-E66E-4546-90B0-7ED937AC2371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A381D62-5537-704A-813F-D536EC3BA9DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="660" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13360" yWindow="2680" windowWidth="30480" windowHeight="25440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Caribbean_frogs_distribution_da" sheetId="1" r:id="rId1"/>
@@ -926,7 +926,7 @@
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -963,7 +963,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -997,7 +997,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
@@ -1099,7 +1099,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1184,7 +1184,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" t="s">
         <v>12</v>
@@ -1269,7 +1269,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D20" t="s">
         <v>12</v>
@@ -1286,7 +1286,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21" t="s">
         <v>12</v>
@@ -1354,7 +1354,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D25" t="s">
         <v>19</v>
@@ -1371,7 +1371,7 @@
         <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D26" t="s">
         <v>12</v>
@@ -1388,7 +1388,7 @@
         <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D27" t="s">
         <v>12</v>
@@ -1439,7 +1439,7 @@
         <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D30" t="s">
         <v>12</v>
@@ -1456,7 +1456,7 @@
         <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D31" t="s">
         <v>12</v>
@@ -1507,7 +1507,7 @@
         <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D34" t="s">
         <v>12</v>
@@ -1524,7 +1524,7 @@
         <v>34</v>
       </c>
       <c r="C35" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D35" t="s">
         <v>12</v>
@@ -1541,7 +1541,7 @@
         <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D36" t="s">
         <v>12</v>
@@ -1592,7 +1592,7 @@
         <v>38</v>
       </c>
       <c r="C39" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D39" t="s">
         <v>12</v>
@@ -1609,7 +1609,7 @@
         <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D40" t="s">
         <v>12</v>
@@ -1626,7 +1626,7 @@
         <v>40</v>
       </c>
       <c r="C41" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D41" t="s">
         <v>12</v>
@@ -1643,7 +1643,7 @@
         <v>41</v>
       </c>
       <c r="C42" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D42" t="s">
         <v>12</v>
@@ -1660,7 +1660,7 @@
         <v>42</v>
       </c>
       <c r="C43" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D43" t="s">
         <v>12</v>
@@ -1677,7 +1677,7 @@
         <v>43</v>
       </c>
       <c r="C44" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D44" t="s">
         <v>12</v>
@@ -1711,7 +1711,7 @@
         <v>45</v>
       </c>
       <c r="C46" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D46" t="s">
         <v>12</v>
@@ -1728,7 +1728,7 @@
         <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D47" t="s">
         <v>12</v>
@@ -1745,7 +1745,7 @@
         <v>47</v>
       </c>
       <c r="C48" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D48" t="s">
         <v>12</v>
@@ -1762,7 +1762,7 @@
         <v>48</v>
       </c>
       <c r="C49" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D49" t="s">
         <v>12</v>
@@ -1813,7 +1813,7 @@
         <v>51</v>
       </c>
       <c r="C52" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D52" t="s">
         <v>12</v>
@@ -1830,7 +1830,7 @@
         <v>52</v>
       </c>
       <c r="C53" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D53" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
changes following Yang's comments
</commit_message>
<xml_diff>
--- a/data/Insula_checklist.xlsx
+++ b/data/Insula_checklist.xlsx
@@ -5,25 +5,25 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Luis/Desktop/GIT_R_CODE/LearnDAISIEprep/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Luis/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDCAE45F-D3D7-0342-98C9-061A6A8DEF42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0392A304-2A73-1248-88EF-C15DF9E07BDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13360" yWindow="2680" windowWidth="30480" windowHeight="25440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4100" yWindow="22280" windowWidth="29920" windowHeight="18660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Caribbean_beet_distribution_da" sheetId="1" r:id="rId1"/>
+    <sheet name="Caribbean_Insula" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Caribbean_beet_distribution_da!$A$1:$E$54</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Caribbean_Insula!$A$1:$E$54</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="24">
   <si>
     <t>Island</t>
   </si>
@@ -52,44 +52,56 @@
     <t>Species</t>
   </si>
   <si>
+    <t>Endemicity_status</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Sampled in phylogeny</t>
+  </si>
+  <si>
+    <t>Endemic to Jamaica</t>
+  </si>
+  <si>
+    <t>Endemic to Bahamas</t>
+  </si>
+  <si>
+    <t>Endemic to Cuba</t>
+  </si>
+  <si>
+    <t>Endemic to Hispaniola</t>
+  </si>
+  <si>
+    <t>Endemic to Lesser Antilles</t>
+  </si>
+  <si>
+    <t>Endemic to Puerto Rico</t>
+  </si>
+  <si>
+    <t>Non-endemic (Jamaica and other islands)</t>
+  </si>
+  <si>
+    <t>Recently diverged from Jamaican species 42, not sampled</t>
+  </si>
+  <si>
+    <t>Recently discovered, not sampled, closely related to Cuban Species 36 and 37</t>
+  </si>
+  <si>
+    <t>Not sampled, very similiar to mainland species 21, 22, 23. Found on Jamaica but not closely related to other Jamaican species</t>
+  </si>
+  <si>
     <t>Taxon</t>
   </si>
   <si>
     <t>Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Species </t>
-  </si>
-  <si>
-    <t>Endemic</t>
-  </si>
-  <si>
-    <t>Endemicity_status</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Sampled in phylogeny</t>
-  </si>
-  <si>
-    <t>Recently discovered, not sampled, closely related to Species 36 and 37</t>
-  </si>
-  <si>
-    <t>Recently split from species 42, not sampled</t>
-  </si>
-  <si>
-    <t>Non-endemic</t>
-  </si>
-  <si>
-    <t>Not sampled, very similiar to mainland species 21, 22, 23. Not closely related to other Jamaican species</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -220,6 +232,12 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -566,8 +584,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -925,34 +944,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="89.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -966,10 +985,10 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -983,10 +1002,10 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1000,10 +1019,10 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1017,10 +1036,10 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1034,10 +1053,10 @@
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1051,10 +1070,10 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1068,10 +1087,10 @@
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1085,10 +1104,10 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1105,7 +1124,7 @@
         <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1119,10 +1138,10 @@
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E11" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1136,10 +1155,10 @@
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E12" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -1153,10 +1172,10 @@
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E13" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1170,10 +1189,10 @@
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E14" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1187,10 +1206,10 @@
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E15" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -1204,10 +1223,10 @@
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E16" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1221,10 +1240,10 @@
         <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E17" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1238,10 +1257,10 @@
         <v>3</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E18" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1255,10 +1274,10 @@
         <v>3</v>
       </c>
       <c r="D19" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E19" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1275,7 +1294,7 @@
         <v>12</v>
       </c>
       <c r="E20" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1289,10 +1308,10 @@
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E21" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -1306,10 +1325,10 @@
         <v>7</v>
       </c>
       <c r="D22" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -1323,10 +1342,10 @@
         <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E23" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1340,10 +1359,10 @@
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -1360,7 +1379,7 @@
         <v>18</v>
       </c>
       <c r="E25" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -1377,7 +1396,7 @@
         <v>12</v>
       </c>
       <c r="E26" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -1394,7 +1413,7 @@
         <v>12</v>
       </c>
       <c r="E27" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -1408,10 +1427,10 @@
         <v>3</v>
       </c>
       <c r="D28" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E28" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1425,10 +1444,10 @@
         <v>3</v>
       </c>
       <c r="D29" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E29" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -1445,7 +1464,7 @@
         <v>12</v>
       </c>
       <c r="E30" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -1459,10 +1478,10 @@
         <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E31" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -1476,10 +1495,10 @@
         <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E32" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -1493,10 +1512,10 @@
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E33" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -1513,7 +1532,7 @@
         <v>12</v>
       </c>
       <c r="E34" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -1527,10 +1546,10 @@
         <v>2</v>
       </c>
       <c r="D35" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E35" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -1544,10 +1563,10 @@
         <v>2</v>
       </c>
       <c r="D36" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E36" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -1561,10 +1580,10 @@
         <v>3</v>
       </c>
       <c r="D37" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E37" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -1578,10 +1597,10 @@
         <v>3</v>
       </c>
       <c r="D38" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E38" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -1598,7 +1617,7 @@
         <v>12</v>
       </c>
       <c r="E39" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -1615,7 +1634,7 @@
         <v>12</v>
       </c>
       <c r="E40" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -1632,7 +1651,7 @@
         <v>12</v>
       </c>
       <c r="E41" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -1649,7 +1668,7 @@
         <v>12</v>
       </c>
       <c r="E42" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -1666,7 +1685,7 @@
         <v>12</v>
       </c>
       <c r="E43" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -1683,7 +1702,7 @@
         <v>12</v>
       </c>
       <c r="E44" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -1697,10 +1716,10 @@
         <v>3</v>
       </c>
       <c r="D45" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E45" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -1714,10 +1733,10 @@
         <v>2</v>
       </c>
       <c r="D46" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E46" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -1731,10 +1750,10 @@
         <v>2</v>
       </c>
       <c r="D47" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E47" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -1751,7 +1770,7 @@
         <v>12</v>
       </c>
       <c r="E48" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -1768,7 +1787,7 @@
         <v>12</v>
       </c>
       <c r="E49" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -1782,10 +1801,10 @@
         <v>3</v>
       </c>
       <c r="D50" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E50" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -1799,15 +1818,15 @@
         <v>3</v>
       </c>
       <c r="D51" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E51" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B52">
         <v>51</v>
@@ -1819,12 +1838,12 @@
         <v>12</v>
       </c>
       <c r="E52" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B53">
         <v>52</v>
@@ -1836,12 +1855,12 @@
         <v>12</v>
       </c>
       <c r="E53" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B54">
         <v>53</v>
@@ -1850,14 +1869,19 @@
         <v>3</v>
       </c>
       <c r="D54" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E54" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E54" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:E54" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E54">
+      <sortCondition ref="B1:B54"/>
+    </sortState>
+  </autoFilter>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>